<commit_message>
Heuristics database first and second level
</commit_message>
<xml_diff>
--- a/resources/implementation.xlsx
+++ b/resources/implementation.xlsx
@@ -1511,7 +1511,7 @@
         <v>335</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1555,7 +1555,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -1569,7 +1569,7 @@
         <v>335</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1613,7 +1613,7 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1642,7 +1642,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1656,7 +1656,7 @@
         <v>338</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1685,7 +1685,7 @@
         <v>339</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1700,7 +1700,7 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1729,7 +1729,7 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -1743,7 +1743,7 @@
         <v>336</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1772,7 +1772,7 @@
         <v>336</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1787,7 +1787,7 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -1830,7 +1830,7 @@
         <v>335</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1859,7 +1859,7 @@
         <v>335</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1990,7 +1990,7 @@
         <v>0</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -2048,7 +2048,7 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -2106,7 +2106,7 @@
         <v>0</v>
       </c>
       <c r="H23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -2222,7 +2222,7 @@
         <v>0</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -2236,7 +2236,7 @@
         <v>335</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -2309,7 +2309,7 @@
         <v>0</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -2381,7 +2381,7 @@
         <v>340</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -2425,7 +2425,7 @@
         <v>0</v>
       </c>
       <c r="H34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -2454,7 +2454,7 @@
         <v>0</v>
       </c>
       <c r="H35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35">
         <v>0</v>
@@ -2512,7 +2512,7 @@
         <v>0</v>
       </c>
       <c r="H37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -2570,7 +2570,7 @@
         <v>0</v>
       </c>
       <c r="H39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39">
         <v>0</v>
@@ -2599,7 +2599,7 @@
         <v>0</v>
       </c>
       <c r="H40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40">
         <v>0</v>
@@ -2686,7 +2686,7 @@
         <v>0</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43">
         <v>0</v>
@@ -2744,7 +2744,7 @@
         <v>0</v>
       </c>
       <c r="H45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45">
         <v>0</v>
@@ -2802,7 +2802,7 @@
         <v>0</v>
       </c>
       <c r="H47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47">
         <v>0</v>
@@ -2831,7 +2831,7 @@
         <v>0</v>
       </c>
       <c r="H48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I48">
         <v>0</v>
@@ -3005,7 +3005,7 @@
         <v>0</v>
       </c>
       <c r="H54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54">
         <v>0</v>
@@ -3193,7 +3193,7 @@
         <v>344</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -3208,7 +3208,7 @@
         <v>0</v>
       </c>
       <c r="H61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61">
         <v>0</v>
@@ -3222,7 +3222,7 @@
         <v>349</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -3280,7 +3280,7 @@
         <v>349</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -3324,7 +3324,7 @@
         <v>0</v>
       </c>
       <c r="H65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65">
         <v>0</v>
@@ -3338,7 +3338,7 @@
         <v>336</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -3367,7 +3367,7 @@
         <v>341</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -3425,7 +3425,7 @@
         <v>340</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -3440,7 +3440,7 @@
         <v>0</v>
       </c>
       <c r="H69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I69">
         <v>0</v>
@@ -3469,7 +3469,7 @@
         <v>0</v>
       </c>
       <c r="H70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I70">
         <v>0</v>
@@ -3527,7 +3527,7 @@
         <v>0</v>
       </c>
       <c r="H72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I72">
         <v>0</v>
@@ -3614,7 +3614,7 @@
         <v>0</v>
       </c>
       <c r="H75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I75">
         <v>0</v>
@@ -3628,7 +3628,7 @@
         <v>336</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -3643,7 +3643,7 @@
         <v>0</v>
       </c>
       <c r="H76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I76">
         <v>0</v>
@@ -3672,7 +3672,7 @@
         <v>0</v>
       </c>
       <c r="H77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I77">
         <v>0</v>
@@ -3686,7 +3686,7 @@
         <v>335</v>
       </c>
       <c r="C78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -3744,7 +3744,7 @@
         <v>338</v>
       </c>
       <c r="C80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -3802,7 +3802,7 @@
         <v>338</v>
       </c>
       <c r="C82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -3904,7 +3904,7 @@
         <v>0</v>
       </c>
       <c r="H85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I85">
         <v>0</v>
@@ -3918,7 +3918,7 @@
         <v>341</v>
       </c>
       <c r="C86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -3947,7 +3947,7 @@
         <v>339</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -4020,7 +4020,7 @@
         <v>0</v>
       </c>
       <c r="H89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I89">
         <v>0</v>
@@ -4107,7 +4107,7 @@
         <v>0</v>
       </c>
       <c r="H92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I92">
         <v>0</v>
@@ -4194,7 +4194,7 @@
         <v>0</v>
       </c>
       <c r="H95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I95">
         <v>0</v>
@@ -4223,7 +4223,7 @@
         <v>0</v>
       </c>
       <c r="H96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I96">
         <v>0</v>
@@ -4252,7 +4252,7 @@
         <v>0</v>
       </c>
       <c r="H97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I97">
         <v>0</v>
@@ -4339,7 +4339,7 @@
         <v>0</v>
       </c>
       <c r="H100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I100">
         <v>0</v>
@@ -4353,7 +4353,7 @@
         <v>336</v>
       </c>
       <c r="C101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -4368,7 +4368,7 @@
         <v>0</v>
       </c>
       <c r="H101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I101">
         <v>0</v>
@@ -4379,7 +4379,7 @@
         <v>109</v>
       </c>
       <c r="C102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -4423,7 +4423,7 @@
         <v>0</v>
       </c>
       <c r="H103">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I103">
         <v>0</v>
@@ -4452,7 +4452,7 @@
         <v>0</v>
       </c>
       <c r="H104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I104">
         <v>0</v>
@@ -4481,7 +4481,7 @@
         <v>0</v>
       </c>
       <c r="H105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I105">
         <v>0</v>
@@ -4524,7 +4524,7 @@
         <v>340</v>
       </c>
       <c r="C107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D107">
         <v>0</v>
@@ -4640,7 +4640,7 @@
         <v>340</v>
       </c>
       <c r="C111">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D111">
         <v>0</v>
@@ -4655,7 +4655,7 @@
         <v>0</v>
       </c>
       <c r="H111">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I111">
         <v>0</v>
@@ -4684,7 +4684,7 @@
         <v>0</v>
       </c>
       <c r="H112">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I112">
         <v>0</v>
@@ -4698,7 +4698,7 @@
         <v>336</v>
       </c>
       <c r="C113">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D113">
         <v>0</v>
@@ -4742,7 +4742,7 @@
         <v>0</v>
       </c>
       <c r="H114">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I114">
         <v>0</v>
@@ -4756,7 +4756,7 @@
         <v>336</v>
       </c>
       <c r="C115">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D115">
         <v>0</v>
@@ -4785,7 +4785,7 @@
         <v>336</v>
       </c>
       <c r="C116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D116">
         <v>0</v>
@@ -4814,7 +4814,7 @@
         <v>335</v>
       </c>
       <c r="C117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D117">
         <v>0</v>
@@ -4916,7 +4916,7 @@
         <v>0</v>
       </c>
       <c r="H120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I120">
         <v>0</v>
@@ -4945,7 +4945,7 @@
         <v>0</v>
       </c>
       <c r="H121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I121">
         <v>0</v>
@@ -5017,7 +5017,7 @@
         <v>349</v>
       </c>
       <c r="C124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D124">
         <v>0</v>
@@ -5119,7 +5119,7 @@
         <v>0</v>
       </c>
       <c r="H127">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I127">
         <v>0</v>
@@ -5177,7 +5177,7 @@
         <v>0</v>
       </c>
       <c r="H129">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I129">
         <v>0</v>
@@ -5249,7 +5249,7 @@
         <v>350</v>
       </c>
       <c r="C132">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D132">
         <v>0</v>
@@ -5307,7 +5307,7 @@
         <v>336</v>
       </c>
       <c r="C134">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D134">
         <v>0</v>
@@ -5351,7 +5351,7 @@
         <v>0</v>
       </c>
       <c r="H135">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I135">
         <v>0</v>
@@ -5394,7 +5394,7 @@
         <v>336</v>
       </c>
       <c r="C137">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D137">
         <v>0</v>
@@ -5496,7 +5496,7 @@
         <v>0</v>
       </c>
       <c r="H140">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I140">
         <v>0</v>
@@ -5525,7 +5525,7 @@
         <v>0</v>
       </c>
       <c r="H141">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I141">
         <v>0</v>
@@ -5568,7 +5568,7 @@
         <v>336</v>
       </c>
       <c r="C143">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D143">
         <v>0</v>
@@ -5641,7 +5641,7 @@
         <v>0</v>
       </c>
       <c r="H145">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I145">
         <v>0</v>
@@ -5699,7 +5699,7 @@
         <v>0</v>
       </c>
       <c r="H147">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I147">
         <v>0</v>
@@ -5713,7 +5713,7 @@
         <v>343</v>
       </c>
       <c r="C148">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D148">
         <v>0</v>
@@ -5757,7 +5757,7 @@
         <v>0</v>
       </c>
       <c r="H149">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I149">
         <v>0</v>
@@ -5829,7 +5829,7 @@
         <v>351</v>
       </c>
       <c r="C152">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D152">
         <v>0</v>
@@ -5858,7 +5858,7 @@
         <v>351</v>
       </c>
       <c r="C153">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D153">
         <v>0</v>
@@ -5873,7 +5873,7 @@
         <v>0</v>
       </c>
       <c r="H153">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I153">
         <v>0</v>
@@ -5887,7 +5887,7 @@
         <v>340</v>
       </c>
       <c r="C154">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D154">
         <v>0</v>
@@ -5902,7 +5902,7 @@
         <v>0</v>
       </c>
       <c r="H154">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I154">
         <v>0</v>
@@ -5974,7 +5974,7 @@
         <v>351</v>
       </c>
       <c r="C157">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D157">
         <v>0</v>
@@ -6018,7 +6018,7 @@
         <v>0</v>
       </c>
       <c r="H158">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I158">
         <v>0</v>
@@ -6047,7 +6047,7 @@
         <v>0</v>
       </c>
       <c r="H159">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I159">
         <v>0</v>
@@ -6076,7 +6076,7 @@
         <v>0</v>
       </c>
       <c r="H160">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I160">
         <v>0</v>
@@ -6163,7 +6163,7 @@
         <v>0</v>
       </c>
       <c r="H163">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I163">
         <v>0</v>
@@ -6206,7 +6206,7 @@
         <v>340</v>
       </c>
       <c r="C165">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D165">
         <v>0</v>
@@ -6308,7 +6308,7 @@
         <v>0</v>
       </c>
       <c r="H168">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I168">
         <v>0</v>
@@ -6351,7 +6351,7 @@
         <v>351</v>
       </c>
       <c r="C170">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D170">
         <v>0</v>
@@ -6380,7 +6380,7 @@
         <v>349</v>
       </c>
       <c r="C171">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D171">
         <v>0</v>
@@ -6395,7 +6395,7 @@
         <v>0</v>
       </c>
       <c r="H171">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I171">
         <v>0</v>
@@ -6424,7 +6424,7 @@
         <v>0</v>
       </c>
       <c r="H172">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I172">
         <v>0</v>
@@ -6467,7 +6467,7 @@
         <v>340</v>
       </c>
       <c r="C174">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D174">
         <v>0</v>
@@ -6496,7 +6496,7 @@
         <v>339</v>
       </c>
       <c r="C175">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D175">
         <v>0</v>
@@ -6525,7 +6525,7 @@
         <v>340</v>
       </c>
       <c r="C176">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D176">
         <v>0</v>
@@ -6554,7 +6554,7 @@
         <v>343</v>
       </c>
       <c r="C177">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D177">
         <v>0</v>
@@ -6612,7 +6612,7 @@
         <v>336</v>
       </c>
       <c r="C179">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D179">
         <v>0</v>
@@ -6728,7 +6728,7 @@
         <v>352</v>
       </c>
       <c r="C183">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D183">
         <v>0</v>
@@ -6859,7 +6859,7 @@
         <v>0</v>
       </c>
       <c r="H187">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I187">
         <v>0</v>
@@ -6917,7 +6917,7 @@
         <v>0</v>
       </c>
       <c r="H189">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I189">
         <v>0</v>
@@ -6931,7 +6931,7 @@
         <v>336</v>
       </c>
       <c r="C190">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D190">
         <v>0</v>
@@ -6960,7 +6960,7 @@
         <v>336</v>
       </c>
       <c r="C191">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D191">
         <v>0</v>
@@ -7018,7 +7018,7 @@
         <v>337</v>
       </c>
       <c r="C193">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D193">
         <v>0</v>
@@ -7076,7 +7076,7 @@
         <v>349</v>
       </c>
       <c r="C195">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D195">
         <v>0</v>
@@ -7105,7 +7105,7 @@
         <v>345</v>
       </c>
       <c r="C196">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D196">
         <v>0</v>
@@ -7134,7 +7134,7 @@
         <v>349</v>
       </c>
       <c r="C197">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D197">
         <v>0</v>
@@ -7149,7 +7149,7 @@
         <v>0</v>
       </c>
       <c r="H197">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I197">
         <v>0</v>
@@ -7178,7 +7178,7 @@
         <v>0</v>
       </c>
       <c r="H198">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I198">
         <v>0</v>
@@ -7207,7 +7207,7 @@
         <v>0</v>
       </c>
       <c r="H199">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I199">
         <v>0</v>
@@ -7221,7 +7221,7 @@
         <v>340</v>
       </c>
       <c r="C200">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D200">
         <v>0</v>
@@ -7352,7 +7352,7 @@
         <v>0</v>
       </c>
       <c r="H204">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I204">
         <v>0</v>
@@ -7395,7 +7395,7 @@
         <v>345</v>
       </c>
       <c r="C206">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D206">
         <v>0</v>
@@ -7410,7 +7410,7 @@
         <v>0</v>
       </c>
       <c r="H206">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I206">
         <v>0</v>
@@ -7424,7 +7424,7 @@
         <v>343</v>
       </c>
       <c r="C207">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D207">
         <v>0</v>
@@ -7482,7 +7482,7 @@
         <v>336</v>
       </c>
       <c r="C209">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D209">
         <v>0</v>
@@ -7555,7 +7555,7 @@
         <v>0</v>
       </c>
       <c r="H211">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I211">
         <v>0</v>
@@ -7714,7 +7714,7 @@
         <v>336</v>
       </c>
       <c r="C217">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D217">
         <v>0</v>
@@ -7729,7 +7729,7 @@
         <v>0</v>
       </c>
       <c r="H217">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I217">
         <v>0</v>
@@ -7772,7 +7772,7 @@
         <v>343</v>
       </c>
       <c r="C219">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D219">
         <v>0</v>
@@ -7830,7 +7830,7 @@
         <v>334</v>
       </c>
       <c r="C221">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D221">
         <v>0</v>
@@ -7845,7 +7845,7 @@
         <v>0</v>
       </c>
       <c r="H221">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I221">
         <v>0</v>
@@ -7874,7 +7874,7 @@
         <v>0</v>
       </c>
       <c r="H222">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I222">
         <v>0</v>
@@ -7903,7 +7903,7 @@
         <v>0</v>
       </c>
       <c r="H223">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I223">
         <v>0</v>
@@ -7917,7 +7917,7 @@
         <v>335</v>
       </c>
       <c r="C224">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D224">
         <v>0</v>
@@ -7932,7 +7932,7 @@
         <v>0</v>
       </c>
       <c r="H224">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I224">
         <v>0</v>
@@ -8048,7 +8048,7 @@
         <v>0</v>
       </c>
       <c r="H228">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I228">
         <v>0</v>
@@ -8077,7 +8077,7 @@
         <v>0</v>
       </c>
       <c r="H229">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I229">
         <v>0</v>
@@ -8106,7 +8106,7 @@
         <v>0</v>
       </c>
       <c r="H230">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I230">
         <v>0</v>
@@ -8193,7 +8193,7 @@
         <v>0</v>
       </c>
       <c r="H233">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I233">
         <v>0</v>
@@ -8236,7 +8236,7 @@
         <v>336</v>
       </c>
       <c r="C235">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D235">
         <v>0</v>
@@ -8265,7 +8265,7 @@
         <v>336</v>
       </c>
       <c r="C236">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D236">
         <v>0</v>
@@ -8425,7 +8425,7 @@
         <v>0</v>
       </c>
       <c r="H241">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I241">
         <v>0</v>
@@ -8483,7 +8483,7 @@
         <v>0</v>
       </c>
       <c r="H243">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I243">
         <v>0</v>
@@ -8497,7 +8497,7 @@
         <v>340</v>
       </c>
       <c r="C244">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D244">
         <v>0</v>
@@ -8526,7 +8526,7 @@
         <v>335</v>
       </c>
       <c r="C245">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D245">
         <v>0</v>
@@ -8570,7 +8570,7 @@
         <v>0</v>
       </c>
       <c r="H246">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I246">
         <v>0</v>
@@ -8628,7 +8628,7 @@
         <v>0</v>
       </c>
       <c r="H248">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I248">
         <v>0</v>
@@ -8642,7 +8642,7 @@
         <v>340</v>
       </c>
       <c r="C249">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D249">
         <v>0</v>
@@ -8671,7 +8671,7 @@
         <v>335</v>
       </c>
       <c r="C250">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D250">
         <v>0</v>
@@ -8715,7 +8715,7 @@
         <v>0</v>
       </c>
       <c r="H251">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I251">
         <v>0</v>
@@ -8729,7 +8729,7 @@
         <v>340</v>
       </c>
       <c r="C252">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D252">
         <v>0</v>
@@ -8758,7 +8758,7 @@
         <v>336</v>
       </c>
       <c r="C253">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D253">
         <v>0</v>
@@ -8773,7 +8773,7 @@
         <v>0</v>
       </c>
       <c r="H253">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I253">
         <v>0</v>
@@ -8845,7 +8845,7 @@
         <v>345</v>
       </c>
       <c r="C256">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D256">
         <v>0</v>
@@ -8932,7 +8932,7 @@
         <v>343</v>
       </c>
       <c r="C259">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D259">
         <v>0</v>
@@ -8947,7 +8947,7 @@
         <v>0</v>
       </c>
       <c r="H259">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I259">
         <v>0</v>
@@ -9063,7 +9063,7 @@
         <v>0</v>
       </c>
       <c r="H263">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I263">
         <v>0</v>
@@ -9077,7 +9077,7 @@
         <v>345</v>
       </c>
       <c r="C264">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D264">
         <v>0</v>
@@ -9135,7 +9135,7 @@
         <v>343</v>
       </c>
       <c r="C266">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D266">
         <v>0</v>
@@ -9164,7 +9164,7 @@
         <v>343</v>
       </c>
       <c r="C267">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D267">
         <v>0</v>
@@ -9193,7 +9193,7 @@
         <v>338</v>
       </c>
       <c r="C268">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D268">
         <v>0</v>
@@ -9237,7 +9237,7 @@
         <v>0</v>
       </c>
       <c r="H269">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I269">
         <v>0</v>
@@ -9280,7 +9280,7 @@
         <v>340</v>
       </c>
       <c r="C271">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D271">
         <v>0</v>
@@ -9295,7 +9295,7 @@
         <v>0</v>
       </c>
       <c r="H271">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I271">
         <v>0</v>
@@ -9353,7 +9353,7 @@
         <v>0</v>
       </c>
       <c r="H273">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I273">
         <v>0</v>
@@ -9382,7 +9382,7 @@
         <v>0</v>
       </c>
       <c r="H274">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I274">
         <v>0</v>
@@ -9411,7 +9411,7 @@
         <v>0</v>
       </c>
       <c r="H275">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I275">
         <v>0</v>
@@ -9425,7 +9425,7 @@
         <v>345</v>
       </c>
       <c r="C276">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D276">
         <v>0</v>
@@ -9440,7 +9440,7 @@
         <v>0</v>
       </c>
       <c r="H276">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I276">
         <v>0</v>
@@ -9585,7 +9585,7 @@
         <v>0</v>
       </c>
       <c r="H281">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I281">
         <v>0</v>
@@ -9686,7 +9686,7 @@
         <v>341</v>
       </c>
       <c r="C285">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D285">
         <v>0</v>
@@ -9701,7 +9701,7 @@
         <v>0</v>
       </c>
       <c r="H285">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I285">
         <v>0</v>
@@ -9875,7 +9875,7 @@
         <v>0</v>
       </c>
       <c r="H291">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I291">
         <v>0</v>
@@ -9904,7 +9904,7 @@
         <v>0</v>
       </c>
       <c r="H292">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I292">
         <v>0</v>
@@ -9918,7 +9918,7 @@
         <v>351</v>
       </c>
       <c r="C293">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D293">
         <v>0</v>
@@ -10092,7 +10092,7 @@
         <v>334</v>
       </c>
       <c r="C299">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D299">
         <v>0</v>
@@ -10150,7 +10150,7 @@
         <v>336</v>
       </c>
       <c r="C301">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D301">
         <v>0</v>
@@ -10165,7 +10165,7 @@
         <v>0</v>
       </c>
       <c r="H301">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I301">
         <v>0</v>
@@ -10208,7 +10208,7 @@
         <v>349</v>
       </c>
       <c r="C303">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D303">
         <v>0</v>
@@ -10223,7 +10223,7 @@
         <v>0</v>
       </c>
       <c r="H303">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I303">
         <v>0</v>
@@ -10324,7 +10324,7 @@
         <v>338</v>
       </c>
       <c r="C307">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D307">
         <v>0</v>
@@ -10353,7 +10353,7 @@
         <v>335</v>
       </c>
       <c r="C308">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D308">
         <v>0</v>
@@ -10368,7 +10368,7 @@
         <v>0</v>
       </c>
       <c r="H308">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I308">
         <v>0</v>
@@ -10382,7 +10382,7 @@
         <v>336</v>
       </c>
       <c r="C309">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D309">
         <v>0</v>
@@ -10426,7 +10426,7 @@
         <v>0</v>
       </c>
       <c r="H310">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I310">
         <v>0</v>
@@ -10455,7 +10455,7 @@
         <v>0</v>
       </c>
       <c r="H311">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I311">
         <v>0</v>
@@ -10571,7 +10571,7 @@
         <v>0</v>
       </c>
       <c r="H315">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I315">
         <v>0</v>
@@ -10600,7 +10600,7 @@
         <v>0</v>
       </c>
       <c r="H316">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I316">
         <v>0</v>
@@ -10629,7 +10629,7 @@
         <v>0</v>
       </c>
       <c r="H317">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I317">
         <v>0</v>
@@ -10672,7 +10672,7 @@
         <v>336</v>
       </c>
       <c r="C319">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D319">
         <v>0</v>
@@ -10687,7 +10687,7 @@
         <v>0</v>
       </c>
       <c r="H319">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I319">
         <v>0</v>
@@ -10774,7 +10774,7 @@
         <v>0</v>
       </c>
       <c r="H322">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I322">
         <v>0</v>
@@ -10832,7 +10832,7 @@
         <v>0</v>
       </c>
       <c r="H324">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I324">
         <v>0</v>
@@ -10861,7 +10861,7 @@
         <v>0</v>
       </c>
       <c r="H325">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I325">
         <v>0</v>
@@ -10875,7 +10875,7 @@
         <v>336</v>
       </c>
       <c r="C326">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D326">
         <v>0</v>
@@ -10904,7 +10904,7 @@
         <v>336</v>
       </c>
       <c r="C327">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D327">
         <v>0</v>
@@ -10977,7 +10977,7 @@
         <v>0</v>
       </c>
       <c r="H329">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I329">
         <v>0</v>

</xml_diff>